<commit_message>
Affichage/Disparition gif scroll down OK
</commit_message>
<xml_diff>
--- a/projet.xlsx
+++ b/projet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EDD1D6-672D-41FA-B843-D22452C04B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3C2EE5-72C0-4F14-AD66-9CD2F1F062CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E3580C5A-1EED-4EC5-B638-3012E505D781}"/>
   </bookViews>
@@ -40,17 +40,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
   <si>
     <t>debut : effect site las vegas parano</t>
   </si>
   <si>
-    <t>Effet glitch chargement des images</t>
-  </si>
-  <si>
-    <t>    Liste des compétences (Java, Python, Linux, Docker...)</t>
-  </si>
-  <si>
     <t>## Cursor</t>
   </si>
   <si>
@@ -138,30 +132,18 @@
     <t>cfcf39</t>
   </si>
   <si>
-    <t>Au scroll des obj qui motent à un rythme différents</t>
-  </si>
-  <si>
-    <t>Pq pas des obj 3d qu'on peut nous aussi faire tourner</t>
-  </si>
-  <si>
     <t>Thème/mood : Cowboy Bebop =&gt; espace, blues, western</t>
   </si>
   <si>
     <t>Menu comme mec stylé</t>
   </si>
   <si>
-    <t>Afficher une image du projet au passe de la souris, où ?</t>
-  </si>
-  <si>
     <t>Affichage liste projets</t>
   </si>
   <si>
     <t>Popup projet</t>
   </si>
   <si>
-    <t>Autres info à présenter</t>
-  </si>
-  <si>
     <t>Fusée qui passe/se deplace au scroll</t>
   </si>
   <si>
@@ -198,9 +180,6 @@
     <t>Fond noir dans les etoiles</t>
   </si>
   <si>
-    <t>Replissage text</t>
-  </si>
-  <si>
     <t>https://custom-hover-animations.webflow.io/</t>
   </si>
   <si>
@@ -216,26 +195,86 @@
     <t>Crédit couleur suivante</t>
   </si>
   <si>
-    <t>Voir auter pour dimensions, pas contrôle…</t>
-  </si>
-  <si>
     <t>Réorganiser projets : 1 photo principale, et autres</t>
   </si>
   <si>
-    <t>lottie pour scroll down</t>
-  </si>
-  <si>
-    <t>Finir font</t>
-  </si>
-  <si>
     <t>Text trop sur le cote en mode tel</t>
+  </si>
+  <si>
+    <t>Compétences</t>
+  </si>
+  <si>
+    <t>Crédits</t>
+  </si>
+  <si>
+    <t>Valider l'animation de la fusée : vers le haut ?</t>
+  </si>
+  <si>
+    <t>Comment organiser le text et les photos : inspiration CowboyBebop</t>
+  </si>
+  <si>
+    <t>Photo : comme panneau pub en ville, photos à la palce des affiches</t>
+  </si>
+  <si>
+    <t>Effet glitch chargement des images ?</t>
+  </si>
+  <si>
+    <t>Liste des compétences (Java, Python, Linux, Docker...)</t>
+  </si>
+  <si>
+    <t>Pour chaque compétence, liste des projets ?</t>
+  </si>
+  <si>
+    <t>Cette partie importante pour les recrutements</t>
+  </si>
+  <si>
+    <t>Bouton menu pour les différentes parties</t>
+  </si>
+  <si>
+    <t>Autres points</t>
+  </si>
+  <si>
+    <t>Inspirtation Cowboy Bebop</t>
+  </si>
+  <si>
+    <t>Nom ? Prenom, linkedin, github, année, sources ?</t>
+  </si>
+  <si>
+    <t>Déplacementt etoiles au scroll, effet on se déplace vraiment</t>
+  </si>
+  <si>
+    <t>Affiche image principale du projet</t>
+  </si>
+  <si>
+    <t>Affichage noms des projets, GIF intro en fond</t>
+  </si>
+  <si>
+    <t>Hover</t>
+  </si>
+  <si>
+    <t>Remplissage du text, du fond ? Pour bien différencier, et permet ouvrir popup</t>
+  </si>
+  <si>
+    <t>Effet granuleux bleu et noire commme intro, sur les photos</t>
+  </si>
+  <si>
+    <t>Rendre propre l'animation des traits jaunes, dimensions</t>
+  </si>
+  <si>
+    <t>https://www.google.com/search?sca_esv=12ce420749b4de42&amp;rlz=1C1ONGR_frFR1087FR1087&amp;sxsrf=ADLYWIJosQwkrGhtIVAdQhWgVkCiAZUHyA:1730624441515&amp;q=comment+s%27appelle+le+fait+d%27avoir+du+grain+sur+une+photo&amp;udm=2&amp;fbs=AEQNm0CbCVgAZ5mWEJDg6aoPVcBgTlosgQSuzBMlnAdio07UCId2t1azIRgowYJD0nDbqEIN7XYIyS3uBYzHmWPp2pnW1aUeS8cvBgTxtkh0oXYZb9sk4SqfagNzG1TA2KSV_2hYbehaG5o57MYKXrNlP11_11VIo5gzHsHhWWSF5ToeyQTImhU&amp;sa=X&amp;sqi=2&amp;ved=2ahUKEwijxc245r-JAxXWBfsDHeL4N1QQtKgLegQIEhAB&amp;biw=1536&amp;bih=695&amp;dpr=1.25#vhid=NpU694-NCNCKPM&amp;vssid=mosaic</t>
+  </si>
+  <si>
+    <t>lottie pour scroll down : cacher sous la fusée, meilleur qualité</t>
+  </si>
+  <si>
+    <t>Animations avec plusieurs vaisseaux</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -257,6 +296,20 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -314,10 +367,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -341,15 +395,25 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="4"/>
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="10">
@@ -619,8 +683,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1CC663EF-82F0-4E5F-8D07-40563650C98F}" name="Tableau2" displayName="Tableau2" ref="B4:C32" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="B4:C32" xr:uid="{1CC663EF-82F0-4E5F-8D07-40563650C98F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1CC663EF-82F0-4E5F-8D07-40563650C98F}" name="Tableau2" displayName="Tableau2" ref="B4:C65" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="B4:C65" xr:uid="{1CC663EF-82F0-4E5F-8D07-40563650C98F}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{4507D888-A201-42C9-8851-10767375BF0F}" name="Visuel" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{5BEE5D16-D2B6-46F9-98B3-853087747E0F}" name="Sources" dataDxfId="6"/>
@@ -966,16 +1030,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613D1184-73B4-4BB5-9F08-6B0CA0D596D6}">
-  <dimension ref="A2:G55"/>
+  <dimension ref="A2:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="96" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="68.21875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="47" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="41" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.44140625" style="2" bestFit="1" customWidth="1"/>
@@ -985,276 +1049,401 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="14"/>
+      <c r="B2" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="18"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B6" s="12" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1"/>
       <c r="E6" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="11" t="s">
-        <v>32</v>
+      <c r="B7" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="C7" s="1"/>
       <c r="E7" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>58</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C8" s="1"/>
       <c r="E8" s="2" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="12" t="s">
-        <v>51</v>
+      <c r="B9" s="16" t="s">
+        <v>45</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B15" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B18" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>53</v>
-      </c>
+      <c r="B19" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C20" s="15"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="1"/>
+      <c r="B21" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" s="11" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="C23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="B24" s="1"/>
+      <c r="B24" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="1"/>
+      <c r="B25" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="B26" s="1"/>
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="1"/>
       <c r="C28" s="1"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C30" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>42</v>
-      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B31" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B32" s="1" t="s">
-        <v>22</v>
+      <c r="B32" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B34" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B37" s="1"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B39" s="13" t="s">
+        <v>53</v>
+      </c>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B41" s="1" t="s">
+        <v>61</v>
+      </c>
       <c r="C41" s="1"/>
     </row>
-    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="1"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C43" s="1"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B45" s="1"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B49" s="1"/>
+      <c r="C49" s="1"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B50" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="1"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B51" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C51" s="1"/>
+    </row>
+    <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>54</v>
+      </c>
       <c r="C52" s="1"/>
     </row>
-    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B53" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" s="1"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B54" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="C54" s="1"/>
     </row>
-    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B55" s="1"/>
       <c r="C55" s="1"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B57" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="1"/>
+    </row>
+    <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B58" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C58" s="1"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B59" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B60" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C60" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B61" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B62" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" s="1"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B63" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C63" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B64" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C64" s="1"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B65" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C65" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:C2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C63" r:id="rId1" xr:uid="{DBD216E5-90E0-49C8-BA13-E89879C2D701}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="3">
-    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1285,22 +1474,22 @@
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1321,7 +1510,7 @@
     <row r="3" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B3" s="3"/>
       <c r="G3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
@@ -1330,63 +1519,63 @@
       </c>
       <c r="C4" s="5"/>
       <c r="G4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" s="6"/>
       <c r="G5" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" s="7"/>
       <c r="G6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" s="8"/>
       <c r="G7" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C8" s="9"/>
       <c r="G8" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G9" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G10" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G11" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="G12" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
@@ -1410,7 +1599,7 @@
   <sheetData>
     <row r="2" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add video scroll, delete unusless files, style...
</commit_message>
<xml_diff>
--- a/projet.xlsx
+++ b/projet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3C2EE5-72C0-4F14-AD66-9CD2F1F062CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9130C891-F673-4FBC-8C8A-B6DF995BD773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E3580C5A-1EED-4EC5-B638-3012E505D781}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="83">
   <si>
     <t>debut : effect site las vegas parano</t>
   </si>
@@ -207,9 +207,6 @@
     <t>Crédits</t>
   </si>
   <si>
-    <t>Valider l'animation de la fusée : vers le haut ?</t>
-  </si>
-  <si>
     <t>Comment organiser le text et les photos : inspiration CowboyBebop</t>
   </si>
   <si>
@@ -268,6 +265,30 @@
   </si>
   <si>
     <t>Animations avec plusieurs vaisseaux</t>
+  </si>
+  <si>
+    <t>Valider l'animation de la fusée : vers le haut ? Cacher plus vite</t>
+  </si>
+  <si>
+    <t>Filtre granuleux sur tout le site ?</t>
+  </si>
+  <si>
+    <t>Video qui avance/recule au scroll</t>
+  </si>
+  <si>
+    <t>Avance/recule du GIF en fonction du scroll</t>
+  </si>
+  <si>
+    <t>24/10/2021, 4L trophy, …</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cjhaque projet sa pop up perso ? Scroll video 4l, certain en 3d, jukebox en 3D, </t>
+  </si>
+  <si>
+    <t>Bien intégrer le fait d'avoir des boutons de projets, rester dans le theme avec la photo</t>
+  </si>
+  <si>
+    <t>Le pb est que quand win2 est fini on passe à laz 3, et donc la 2 monte, et les traits jaune pas encore supp se voient</t>
   </si>
 </sst>
 </file>
@@ -398,9 +419,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -409,6 +427,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -1032,15 +1053,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613D1184-73B4-4BB5-9F08-6B0CA0D596D6}">
   <dimension ref="A2:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="83" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="68.21875" style="2" customWidth="1"/>
     <col min="2" max="2" width="68.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.77734375" style="2" customWidth="1"/>
     <col min="4" max="4" width="23.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="43.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5546875" style="2"/>
@@ -1098,7 +1119,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="1"/>
@@ -1108,7 +1129,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="C8" s="1"/>
       <c r="E8" s="2" t="s">
@@ -1116,52 +1137,59 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>45</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
-        <v>66</v>
+      <c r="B10" s="17" t="s">
+        <v>65</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>42</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>44</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="15" t="s">
-        <v>74</v>
+      <c r="B14" s="14" t="s">
+        <v>73</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="15" t="s">
-        <v>62</v>
+      <c r="B15" s="14" t="s">
+        <v>61</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
@@ -1178,19 +1206,21 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C21" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C23" s="1"/>
       <c r="F23" s="1" t="s">
@@ -1199,20 +1229,22 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>81</v>
+      </c>
       <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1240,24 +1272,26 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B35" s="1"/>
+      <c r="B35" s="1" t="s">
+        <v>80</v>
+      </c>
       <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1283,25 +1317,25 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C43" s="1"/>
     </row>
@@ -1358,7 +1392,7 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C54" s="1"/>
     </row>
@@ -1378,7 +1412,7 @@
     </row>
     <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B58" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C58" s="1"/>
     </row>
@@ -1416,21 +1450,23 @@
       <c r="B63" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C63" s="17" t="s">
+      <c r="C63" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C64" s="1"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B65" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C65" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
FEAT open popup animation OK
</commit_message>
<xml_diff>
--- a/projet.xlsx
+++ b/projet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9130C891-F673-4FBC-8C8A-B6DF995BD773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509578F7-9E76-453B-BBC8-4F6D57591CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E3580C5A-1EED-4EC5-B638-3012E505D781}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{E3580C5A-1EED-4EC5-B638-3012E505D781}"/>
   </bookViews>
   <sheets>
     <sheet name="Taches" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
   <si>
     <t>debut : effect site las vegas parano</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Le pb est que quand win2 est fini on passe à laz 3, et donc la 2 monte, et les traits jaune pas encore supp se voient</t>
+  </si>
+  <si>
+    <t>popup s'ouvre en glitch</t>
   </si>
 </sst>
 </file>
@@ -1053,8 +1056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613D1184-73B4-4BB5-9F08-6B0CA0D596D6}">
   <dimension ref="A2:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="83" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="83" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1295,7 +1298,9 @@
       <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B36" s="1"/>
+      <c r="B36" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="C36" s="1"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Text loader increment 1 by 1
</commit_message>
<xml_diff>
--- a/projet.xlsx
+++ b/projet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\426\Web\Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509578F7-9E76-453B-BBC8-4F6D57591CD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A104C16-CEE8-42DF-884F-8E67BA1CEDA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8880" xr2:uid="{E3580C5A-1EED-4EC5-B638-3012E505D781}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{E3580C5A-1EED-4EC5-B638-3012E505D781}"/>
   </bookViews>
   <sheets>
     <sheet name="Taches" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="81">
   <si>
     <t>debut : effect site las vegas parano</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Popup projet</t>
   </si>
   <si>
-    <t>Fusée qui passe/se deplace au scroll</t>
-  </si>
-  <si>
     <t>Faire une zone où le text apparait en "coloriant"</t>
   </si>
   <si>
@@ -162,9 +159,6 @@
     <t>https://buttermax.net/</t>
   </si>
   <si>
-    <t>Titre, hover animlation gsap comme lasvegas</t>
-  </si>
-  <si>
     <t>https://fearandloathinginlasvegas.com/</t>
   </si>
   <si>
@@ -265,9 +259,6 @@
   </si>
   <si>
     <t>Animations avec plusieurs vaisseaux</t>
-  </si>
-  <si>
-    <t>Valider l'animation de la fusée : vers le haut ? Cacher plus vite</t>
   </si>
   <si>
     <t>Filtre granuleux sur tout le site ?</t>
@@ -1056,8 +1047,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{613D1184-73B4-4BB5-9F08-6B0CA0D596D6}">
   <dimension ref="A2:G65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="83" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1083,7 +1074,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>16</v>
@@ -1094,13 +1085,13 @@
     </row>
     <row r="5" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>17</v>
@@ -1110,9 +1101,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="12" t="s">
-        <v>40</v>
-      </c>
+      <c r="B6" s="12"/>
       <c r="C6" s="1"/>
       <c r="E6" s="2" t="s">
         <v>18</v>
@@ -1122,81 +1111,77 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="14" t="s">
-        <v>34</v>
-      </c>
+      <c r="B7" s="14"/>
       <c r="C7" s="1"/>
       <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
-        <v>75</v>
-      </c>
+      <c r="B8" s="11"/>
       <c r="C8" s="1"/>
       <c r="E8" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B9" s="15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B11" s="15" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B12" s="15" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B13" s="15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B14" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B15" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B19" s="13" t="s">
         <v>32</v>
@@ -1209,21 +1194,21 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B23" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C23" s="1"/>
       <c r="F23" s="1" t="s">
@@ -1232,21 +1217,21 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B24" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C26" s="1"/>
     </row>
@@ -1259,7 +1244,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C29" s="1"/>
     </row>
@@ -1275,31 +1260,31 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B32" s="10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C32" s="1"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C33" s="1"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C34" s="1"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C35" s="1"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C36" s="1"/>
     </row>
@@ -1309,38 +1294,38 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
     </row>
     <row r="39" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B39" s="13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C39" s="1"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C40" s="1"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C42" s="1"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C43" s="1"/>
     </row>
@@ -1382,22 +1367,22 @@
     </row>
     <row r="52" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B52" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C52" s="1"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B53" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C53" s="1"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C54" s="1"/>
     </row>
@@ -1417,7 +1402,7 @@
     </row>
     <row r="58" spans="1:3" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B58" s="13" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C58" s="1"/>
     </row>
@@ -1426,7 +1411,7 @@
         <v>24</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1434,7 +1419,7 @@
         <v>20</v>
       </c>
       <c r="C60" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1442,7 +1427,7 @@
         <v>20</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1456,21 +1441,21 @@
         <v>31</v>
       </c>
       <c r="C63" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B64" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C64" s="1"/>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B65" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1530,7 +1515,7 @@
     </row>
     <row r="6" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>